<commit_message>
v0.0.5 fix ImmunizationRecommendation supportingImmunization attribute mustSuport = true
</commit_message>
<xml_diff>
--- a/StructureDefinition-Vaccine-Passport-ImmunizationRecommendation.xlsx
+++ b/StructureDefinition-Vaccine-Passport-ImmunizationRecommendation.xlsx
@@ -746,7 +746,7 @@
     <t>ImmunizationRecommendation.recommendation.supportingImmunization</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Immunization|ImmunizationEvaluation)
+    <t xml:space="preserve">Reference(https://ghit42796.github.io/fhir_test/StructureDefinition-Vaccine-Passport-Immunization)
 </t>
   </si>
   <si>
@@ -5279,7 +5279,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" hidden="true">
+    <row r="40">
       <c r="A40" t="s" s="2">
         <v>232</v>
       </c>
@@ -5289,13 +5289,13 @@
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F40" t="s" s="2">
         <v>42</v>
       </c>
       <c r="G40" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H40" t="s" s="2">
         <v>40</v>

</xml_diff>